<commit_message>
bugs related to field modification and combo list
</commit_message>
<xml_diff>
--- a/Mesh4j/branches/Mesh4j_WHO_Facility/Test Report/bug report(update).xlsx
+++ b/Mesh4j/branches/Mesh4j_WHO_Facility/Test Report/bug report(update).xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Title</t>
   </si>
@@ -152,6 +151,30 @@
   </si>
   <si>
     <t xml:space="preserve">1. Modify "FACILITY_DATA_TABLE_SEC_1.xml" form's combo and text fields in MS Access                                                            2. Synchronize MS Access with Cloud                                                  3. Now chose 'refresh'  from mobile option for receiving the updates                                             </t>
+  </si>
+  <si>
+    <t>Chosen option should be saved properly</t>
+  </si>
+  <si>
+    <t>No option is showed as chosen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Load any form in mobile                     2. Select any option from the option list                                                                   3. Click 'Save and Exit'    </t>
+  </si>
+  <si>
+    <t>Updated data should be showed properly during sychronization in MS Access</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated data are not showing properly. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Load any facility profile in mobile                                                 2. Do any modification in text field and option list                                            3. Click 'Send Now'                                   4. Sync MS Access with Cloud         </t>
+  </si>
+  <si>
+    <t>Combo list selection is not working (ref: SEC_1.xml)</t>
+  </si>
+  <si>
+    <t>Modification not works during synchronization (ref: facility profile)</t>
   </si>
 </sst>
 </file>
@@ -525,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -789,6 +812,68 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
+    </row>
+    <row r="8" spans="1:17" ht="60">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+    </row>
+    <row r="9" spans="1:17" ht="75">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>